<commit_message>
done the last chenges
</commit_message>
<xml_diff>
--- a/data/registrations.xlsx
+++ b/data/registrations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cybersec\ctf_backend\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cybersec\ctf_backend-1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32A1C86-EBFA-41A4-8CCC-CD73250AF7D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB7179F-7ADB-4CF3-B5E8-78B854B04711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1829,8 +1829,8 @@
   <dimension ref="A1:N68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G60" sqref="G60"/>
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N72" sqref="N72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>